<commit_message>
Changed DB schemas and API end point in sheet
</commit_message>
<xml_diff>
--- a/backend/FS_SchemaAndDB_v1.0.xlsx
+++ b/backend/FS_SchemaAndDB_v1.0.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P7111004\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code_Garage\node-shopping-cart\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DB324857-103E-4094-86CC-0329187E26B7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11325" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DB SCHEMA" sheetId="2" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t>Schema Name</t>
   </si>
@@ -102,18 +103,6 @@
     <t>address</t>
   </si>
   <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>reviews</t>
-  </si>
-  <si>
-    <t>[Review]</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>quantity</t>
   </si>
   <si>
@@ -129,36 +118,12 @@
     <t>[Address]</t>
   </si>
   <si>
-    <t>Review</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
-    <t>rating</t>
-  </si>
-  <si>
-    <t>0-5</t>
-  </si>
-  <si>
-    <t>pincode</t>
-  </si>
-  <si>
     <t>products</t>
   </si>
   <si>
-    <t>landmark</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
     <t>Method</t>
   </si>
   <si>
@@ -198,18 +163,12 @@
     <t>Orders</t>
   </si>
   <si>
-    <t>/api/user/order</t>
-  </si>
-  <si>
     <t>To Create a new Order</t>
   </si>
   <si>
     <t xml:space="preserve">To Get All the Orders </t>
   </si>
   <si>
-    <t>/api/user/orderView/:orderId</t>
-  </si>
-  <si>
     <t>To Get Specific Order Details</t>
   </si>
   <si>
@@ -226,12 +185,18 @@
   </si>
   <si>
     <t>Get User Profile</t>
+  </si>
+  <si>
+    <t>/api/user/:userId/orders</t>
+  </si>
+  <si>
+    <t>/api/user/:userId/orderView/:orderId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -632,11 +597,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,7 +704,7 @@
         <v>5</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>20</v>
@@ -762,165 +727,100 @@
         <v>24</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="F8" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="E15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
       <c r="F15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H19" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H20" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -928,11 +828,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,13 +844,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -962,46 +862,46 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1016,69 +916,69 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Registeration service Linked with form
</commit_message>
<xml_diff>
--- a/backend/FS_SchemaAndDB_v1.0.xlsx
+++ b/backend/FS_SchemaAndDB_v1.0.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code_Garage\node-shopping-cart\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FullStackProject\node-shopping-cart_v1\node-shopping-cart\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DB324857-103E-4094-86CC-0329187E26B7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11325" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DB SCHEMA" sheetId="2" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
   <si>
     <t>Schema Name</t>
   </si>
@@ -178,9 +177,6 @@
     <t>Authentication</t>
   </si>
   <si>
-    <t>/api/users/login/:username,:password</t>
-  </si>
-  <si>
     <t>/api/users/profile/:userId</t>
   </si>
   <si>
@@ -191,12 +187,18 @@
   </si>
   <si>
     <t>/api/user/:userId/orderView/:orderId</t>
+  </si>
+  <si>
+    <t>/api/users/login/</t>
+  </si>
+  <si>
+    <t>/api/users/registeration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -597,7 +599,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -828,11 +830,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,7 +928,7 @@
         <v>42</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>45</v>
@@ -937,7 +939,7 @@
         <v>35</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>46</v>
@@ -948,7 +950,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>47</v>
@@ -961,10 +963,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
         <v>49</v>
@@ -975,10 +977,18 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
         <v>51</v>
       </c>
-      <c r="C17" t="s">
-        <v>52</v>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>